<commit_message>
created batch execution suite
</commit_message>
<xml_diff>
--- a/Sportyeez/TestData/TestData.xlsx
+++ b/Sportyeez/TestData/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINIT SINGH\git\Sportyeez\Sportyeez\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E463BC5-AEA4-4C2E-8278-8EA6FB9B9368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACBF881-FFC2-4C77-BADD-8203A47945CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="190" windowWidth="15490" windowHeight="9810" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="190" windowWidth="15490" windowHeight="9810" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
     <sheet name="Manufacturer" sheetId="2" r:id="rId2"/>
+    <sheet name="Retailer" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -175,13 +176,25 @@
     <t>manufacturerManageQuantity</t>
   </si>
   <si>
-    <t>quantityprice</t>
-  </si>
-  <si>
     <t>143</t>
   </si>
   <si>
     <t>pagent</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>retailerLoginTest</t>
+  </si>
+  <si>
+    <t>createAOrder</t>
+  </si>
+  <si>
+    <t>manufacturerAddProductTest</t>
+  </si>
+  <si>
+    <t>manufacturerLoginTest</t>
   </si>
 </sst>
 </file>
@@ -559,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -851,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1794EC-4F92-4673-BE30-E7B41FB6333C}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -879,7 +892,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -913,7 +926,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -945,7 +958,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -956,10 +969,75 @@
         <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4589FEE1-7517-40E7-85DC-7619D7A80863}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>